<commit_message>
QR and adding more context to documentation
</commit_message>
<xml_diff>
--- a/dpp_api/data/Brighteco/parameter_metadata_Brighteco.xlsx
+++ b/dpp_api/data/Brighteco/parameter_metadata_Brighteco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berenicegudino/Desktop/Code/dpp/dpp_app/data/Brighteco/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beren\Code\dpp_smartpass\dpp_app\data\Brighteco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DDEF78-24AD-224C-8632-AC45FF411DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2A1021-2DED-43EB-BD7C-051D04055996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{F5499085-62E6-4B04-A4E2-EEF974C52419}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F5499085-62E6-4B04-A4E2-EEF974C52419}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_metadata" sheetId="4" r:id="rId1"/>
@@ -655,7 +655,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1664,19 +1664,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91110A29-C29E-1746-BC3B-9F1F909FD312}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="48.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="str">
         <f>parameter_metadata_original!A1</f>
         <v>category</v>
@@ -1722,7 +1721,7 @@
         <v>data model definition string</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="str">
         <f>parameter_metadata_original!A2</f>
         <v>1. General product and manufacturer information</v>
@@ -1759,7 +1758,7 @@
         <v>{"DPP Created Timestamp" : {"value":{"@value":"", "@type":"xsd:dateTime"}}}</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="str">
         <f>parameter_metadata_original!A3</f>
         <v>1. General product and manufacturer information</v>
@@ -1800,7 +1799,7 @@
         <v>{"Product ID": {"@type":"gs1:gtin","value": {"@value":"", "@type":"xsd:string"}}}</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="str">
         <f>parameter_metadata_original!A4</f>
         <v>1. General product and manufacturer information</v>
@@ -1837,7 +1836,7 @@
         <v>{"Data carrier type" : {"value":{"@value":"", "@type":"xsd:string"}}}</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="str">
         <f>parameter_metadata_original!A5</f>
         <v>1. General product and manufacturer information</v>
@@ -1874,7 +1873,7 @@
         <v>{"Manufacturing date": {"@type":"gs1:productionDateTime", "value": {"@value":"", "@type":"xsd:dateTime"}}}</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="str">
         <f>parameter_metadata_original!A6</f>
         <v>1. General product and manufacturer information</v>
@@ -1911,7 +1910,7 @@
         <v>{"Manufactured by": {"@type":"gs1:organizationName", "value": {"@value": "", "@type":"xsd:string"}}}</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="str">
         <f>parameter_metadata_original!A7</f>
         <v>1. General product and manufacturer information</v>
@@ -1952,7 +1951,7 @@
         <v>{"Manufacturing place" : {"@type":"gs1:address", "City": {"@type":"gs1:addressLocality", "value":{"@value": "", "@type":"xsd:string"}} , "Address":{"@type":"gs1:streetAddress",  "value":{"@value": "", "@type":"xsd:string"}}}}</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="str">
         <f>parameter_metadata_original!A8</f>
         <v>1. General product and manufacturer information</v>
@@ -1989,7 +1988,7 @@
         <v>{"Product category/group" : {"@type":"gs1:brandName", "value":{"@value":"", "@type":"rdf:langString"}}}</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="str">
         <f>parameter_metadata_original!A9</f>
         <v>1. General product and manufacturer information</v>
@@ -2030,7 +2029,7 @@
         <v>{"Type/Configuration" : {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="str">
         <f>parameter_metadata_original!A10</f>
         <v>1. General product and manufacturer information</v>
@@ -2071,7 +2070,7 @@
         <v>{"Economic operator" : {"@type":"schema:legalName",  "value": {"@value":"", "@type":"xsd:string"}}}</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="str">
         <f>parameter_metadata_original!A15</f>
         <v>1. General product and manufacturer information</v>
@@ -2108,7 +2107,7 @@
         <v>{"Original weight" : {"value":{"@value":"", "@type":"xsd:float", "unitCode":"KGM"}}}</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="str">
         <f>parameter_metadata_original!A16</f>
         <v>1. General product and manufacturer information</v>
@@ -2149,7 +2148,7 @@
         <v>{"Dimensions":{"Height" : {"@type":"gs1:outOfPackageHeight", "value":{"@value":"", "@type":"xsd:float", "unitCode": "MMT"}}, "Width" : {"@type":"gs1:inPackageWidth", "value":{"@value":"", "@type":"xsd:float", "unitCode": "MMT"}}, "Depth" : {"@type":"gs1:inPackageDepth", "value":{"@value":"", "@type":"xsd:float", "unitCode": "MMT"}}}}</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" t="str">
         <f>parameter_metadata_original!A21</f>
         <v>3. Carbon footprint</v>
@@ -2186,7 +2185,7 @@
         <v>{"Carbon footprint (cradle to gate)" : {"value":{"@value":"", "@type":"xsd:float"}}}</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="str">
         <f>parameter_metadata_original!A22</f>
         <v>4. Supply chain due diligence</v>
@@ -2227,7 +2226,7 @@
         <v>{"Information of the due diligence report" : {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="str">
         <f>parameter_metadata_original!A28</f>
         <v>5. Material and composition</v>
@@ -2268,7 +2267,7 @@
         <v>{"Hazardous substances, other than Hg, Cd, Pb" : {"@type":"gs1:ReferencedFileTypeCode-HAZARDOUS_SUBSTANCES_DATA", "value": {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}}</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" t="str">
         <f>parameter_metadata_original!A31</f>
         <v>6. Circularity and resource efficiency</v>
@@ -2305,7 +2304,7 @@
         <v>{"The share of renewable content" : {"value":{"@value":"", "@type":"xsd:float", "unitCode":"P1"}}}</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" t="str">
         <f>parameter_metadata_original!A38</f>
         <v>6. Circularity and resource efficiency</v>
@@ -2346,7 +2345,7 @@
         <v>{"Part numbers for spare parts" : {"value":{"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}}</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" t="str">
         <f>parameter_metadata_original!A39</f>
         <v>6. Circularity and resource efficiency</v>
@@ -2387,7 +2386,7 @@
         <v>{"Information on sources of spare parts" : {"value":{"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}}</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" t="str">
         <f>parameter_metadata_original!A11</f>
         <v>9. Product Updates</v>
@@ -2428,7 +2427,7 @@
         <v>{"Update ID" : { "value": {"@value":"", "@type":"xsd:string"}}}</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" t="str">
         <f>parameter_metadata_original!A12</f>
         <v>9. Product Updates</v>
@@ -2465,7 +2464,7 @@
         <v>{"DPP Update Timestamp" : {"@type":"schema:startTime", "value":{"@type":"schema:DateTime", "value": {"@value":"", "@type":"xsd:dateTime"}}}}</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" t="str">
         <f>parameter_metadata_original!A13</f>
         <v>9. Product Updates</v>
@@ -2502,7 +2501,7 @@
         <v>{"DPP Update Reason" :  {"@type":"schema:description", "value":{"@type":"schema:Text", "value": {"@value":"", "@type":"xsd:string"}}}}</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" t="str">
         <f>parameter_metadata_original!A14</f>
         <v>9. Product Updates</v>
@@ -2539,7 +2538,7 @@
         <v>{"DPP Update Responsible" :  {"@type":"schema:Organization", "value":{"@type":"schema:legalName", "value": {"@value":"", "@type":"xsd:string"}}}}</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" t="str">
         <f>parameter_metadata_original!A17</f>
         <v>9. Product Updates</v>
@@ -2580,7 +2579,7 @@
         <v>{"Color temperature" : {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" t="str">
         <f>parameter_metadata_original!A18</f>
         <v>9. Product Updates</v>
@@ -2621,7 +2620,7 @@
         <v>{"Photometry" : {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" t="str">
         <f>parameter_metadata_original!A19</f>
         <v>9. Product Updates</v>
@@ -2662,7 +2661,7 @@
         <v>{"Datasheet" : {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" t="str">
         <f>parameter_metadata_original!A29</f>
         <v>9. Product Updates</v>
@@ -2703,7 +2702,7 @@
         <v>{"Actual total weight" : {"value":{"@value":"", "@type":"xsd:float", "unitCode":"KGM"}}}</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" t="str">
         <f>parameter_metadata_original!A30</f>
         <v>9. Product Updates</v>
@@ -2744,7 +2743,7 @@
         <v>{"Virgin material weight" : {"value":{"@value":"", "@type":"xsd:float", "unitCode":"KGM"}}}</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" t="str">
         <f>parameter_metadata_original!A32</f>
         <v>9. Product Updates</v>
@@ -2785,7 +2784,7 @@
         <v>{"Recycled content" : {"value":{"@value":"", "@type":"xsd:float", "unitCode":"KGM"}}}</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" t="str">
         <f>parameter_metadata_original!A33</f>
         <v>9. Product Updates</v>
@@ -2822,7 +2821,7 @@
         <v>{"Recycled content [% of original weight]" : {"value":{"@value":"", "@type":"xsd:float",  "unitCode":"P1"}}}</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" t="str">
         <f>parameter_metadata_original!A34</f>
         <v>9. Product Updates</v>
@@ -2859,7 +2858,7 @@
         <v>{"Weight reused components" : {"value":{"@value":"", "@type":"xsd:float", "unitCode":"KGM"}}}</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" t="str">
         <f>parameter_metadata_original!A46</f>
         <v>9. Product Updates</v>
@@ -2900,7 +2899,7 @@
         <v>{"Installation (drawing)" : {"value":{"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}}</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" t="str">
         <f>parameter_metadata_original!A23</f>
         <v>9. Product Updates</v>
@@ -2941,7 +2940,7 @@
         <v>{"Wiring and accessories" : {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" t="str">
         <f>parameter_metadata_original!A24</f>
         <v>9. Product Updates</v>
@@ -2982,7 +2981,7 @@
         <v>{"Electronics and optoelectronics" : {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" t="str">
         <f>parameter_metadata_original!A25</f>
         <v>9. Product Updates</v>
@@ -3023,7 +3022,7 @@
         <v>{"Optical components" : {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" t="str">
         <f>parameter_metadata_original!A26</f>
         <v>9. Product Updates</v>
@@ -3064,7 +3063,7 @@
         <v>{"Drive Components" : {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" t="str">
         <f>parameter_metadata_original!A27</f>
         <v>9. Product Updates</v>
@@ -3105,7 +3104,7 @@
         <v>{"Chassis components" : {"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" t="str">
         <f>parameter_metadata_original!A40</f>
         <v>9. Product Updates</v>
@@ -3146,7 +3145,7 @@
         <v>{"Installation manual" : {"value":{"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}}</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38" t="str">
         <f>parameter_metadata_original!A43</f>
         <v>9. Product Updates</v>
@@ -3183,7 +3182,7 @@
         <v>{"Installation Manager" : {"value":{"@value":"", "@type":"xsd:string"}}}</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39" t="str">
         <f>parameter_metadata_original!A44</f>
         <v>9. Product Updates</v>
@@ -3220,7 +3219,7 @@
         <v>{"Installation address" : {"value":{"@value":"", "@type":"xsd:string"}}}</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" t="str">
         <f>parameter_metadata_original!A45</f>
         <v>9. Product Updates</v>
@@ -3261,7 +3260,7 @@
         <v>{"Installation (where in building)" : {"value":{"@type":"gs1:pip", "value":{"@value":"", "@type":"xsd:anyURI"}}}}</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41" t="str">
         <f>parameter_metadata_original!A35</f>
         <v>9. Product Updates</v>
@@ -3298,7 +3297,7 @@
         <v>{"Waste produced" : {"value":{"@value":"", "@type":"xsd:float", "unitCode":"KGM"}}}</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" t="str">
         <f>parameter_metadata_original!A36</f>
         <v>9. Product Updates</v>
@@ -3335,7 +3334,7 @@
         <v>{"Reusable components (original)" : {"value":{"@value":"", "@type":"xsd:float", "unitCode":"KGM"}}}</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" t="str">
         <f>parameter_metadata_original!A37</f>
         <v>9. Product Updates</v>
@@ -3372,7 +3371,7 @@
         <v>{"Recyclable material (wt%)" : {"value":{"@value":"", "@type":"xsd:float",  "unitCode":"P1"}}}</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44" t="str">
         <f>parameter_metadata_original!A48</f>
         <v>9. Product Updates</v>
@@ -3409,7 +3408,7 @@
         <v>{"Installed capacity" : {"@type":"gs1:Power", "value":{"@value":"", "@type":"xsd:float", "unitCode":"KWH"}}}</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" t="str">
         <f>parameter_metadata_original!A49</f>
         <v>9. Product Updates</v>
@@ -3446,7 +3445,7 @@
         <v>{"Energy usage" : {"@type":"gs1:Power", "value":{"@value":"", "@type":"xsd:float", "unitCode":"KWH"}}}</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" t="str">
         <f>parameter_metadata_original!A50</f>
         <v>9. Product Updates</v>
@@ -3483,7 +3482,7 @@
         <v>{"Energy inherent" : {"@type":"gs1:Power", "value":{"@value":"", "@type":"xsd:float", "unitCode":"3B"}}}</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="A47" t="str">
         <f>parameter_metadata_original!A74</f>
         <v>9. Product Updates</v>
@@ -3545,22 +3544,22 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5" customWidth="1"/>
-    <col min="3" max="3" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="96.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="96.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3595,7 +3594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
@@ -3618,7 +3617,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -3644,7 +3643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -3667,7 +3666,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
         <v>34</v>
       </c>
@@ -3690,7 +3689,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
@@ -3713,7 +3712,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -3739,7 +3738,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -3762,7 +3761,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
@@ -3788,7 +3787,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -3817,7 +3816,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>149</v>
       </c>
@@ -3846,7 +3845,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>149</v>
       </c>
@@ -3869,7 +3868,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -3892,7 +3891,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>149</v>
       </c>
@@ -3921,7 +3920,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -3944,7 +3943,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="60">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -3970,7 +3969,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>149</v>
       </c>
@@ -3996,7 +3995,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>149</v>
       </c>
@@ -4022,7 +4021,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>149</v>
       </c>
@@ -4048,7 +4047,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
@@ -4060,7 +4059,7 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -4083,7 +4082,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -4109,7 +4108,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>149</v>
       </c>
@@ -4135,7 +4134,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -4161,7 +4160,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>149</v>
       </c>
@@ -4187,7 +4186,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>149</v>
       </c>
@@ -4213,7 +4212,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -4239,7 +4238,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" s="4" t="s">
         <v>65</v>
       </c>
@@ -4268,7 +4267,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -4297,7 +4296,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>149</v>
       </c>
@@ -4323,7 +4322,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="4" t="s">
         <v>36</v>
       </c>
@@ -4346,7 +4345,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -4372,7 +4371,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -4395,7 +4394,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>149</v>
       </c>
@@ -4418,7 +4417,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>149</v>
       </c>
@@ -4441,7 +4440,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -4464,7 +4463,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -4487,7 +4486,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -4516,7 +4515,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -4545,7 +4544,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -4571,7 +4570,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>149</v>
       </c>
@@ -4589,7 +4588,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -4603,7 +4602,7 @@
       <c r="G42" s="17"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>149</v>
       </c>
@@ -4626,7 +4625,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>149</v>
       </c>
@@ -4649,7 +4648,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>149</v>
       </c>
@@ -4675,7 +4674,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>149</v>
       </c>
@@ -4701,7 +4700,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -4711,7 +4710,7 @@
       </c>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>149</v>
       </c>
@@ -4734,7 +4733,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>149</v>
       </c>
@@ -4757,7 +4756,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>149</v>
       </c>
@@ -4780,7 +4779,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -4788,7 +4787,7 @@
       <c r="G51" s="17"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -4798,7 +4797,7 @@
       <c r="G52" s="17"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>149</v>
       </c>
@@ -4815,14 +4814,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="D54" s="9" t="s">
         <v>83</v>
       </c>
       <c r="G54" s="17"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>149</v>
       </c>
@@ -4840,7 +4839,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>149</v>
       </c>
@@ -4858,7 +4857,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -4866,7 +4865,7 @@
       <c r="G57" s="17"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>149</v>
       </c>
@@ -4883,7 +4882,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -4895,7 +4894,7 @@
       </c>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -4905,7 +4904,7 @@
       </c>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -4917,7 +4916,7 @@
       </c>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62" t="s">
         <v>149</v>
       </c>
@@ -4934,7 +4933,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>149</v>
       </c>
@@ -4951,7 +4950,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11">
       <c r="A64" t="s">
         <v>149</v>
       </c>
@@ -4969,7 +4968,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11">
       <c r="A65" t="s">
         <v>149</v>
       </c>
@@ -4987,7 +4986,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -5005,7 +5004,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>149</v>
       </c>
@@ -5023,7 +5022,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="A68" t="s">
         <v>149</v>
       </c>
@@ -5041,7 +5040,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>149</v>
       </c>
@@ -5059,7 +5058,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>149</v>
       </c>
@@ -5077,7 +5076,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -5095,7 +5094,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>149</v>
       </c>
@@ -5113,7 +5112,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -5131,7 +5130,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11">
       <c r="A74" t="s">
         <v>149</v>
       </c>
@@ -5176,14 +5175,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.5" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5194,7 +5193,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -5205,7 +5204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -5216,7 +5215,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -5227,7 +5226,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -5238,7 +5237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -5249,7 +5248,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -5273,13 +5272,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5287,7 +5286,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -5295,7 +5294,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -5303,7 +5302,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -5311,7 +5310,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -5319,7 +5318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -5327,7 +5326,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>149</v>
       </c>

</xml_diff>